<commit_message>
E:/Programas/Git/Inscripcion sabe ahora si una lista hay estudiantes de más o menos de los que se necesita para esa categoria
</commit_message>
<xml_diff>
--- a/frontend/public/Plantillas/FormatoParaSubirLista.xlsx
+++ b/frontend/public/Plantillas/FormatoParaSubirLista.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programación\ohsansi\frontend\public\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6416C9E5-6D9F-4671-A8B9-C65BD3CDC1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263E5803-89A4-4C0D-B392-C091466BA7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Nombre</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>N°</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Team: Coloque un mismo número para aquellos estudiantes que hagan grupo en las categorias correspondientes</t>
   </si>
 </sst>
 </file>
@@ -464,7 +470,7 @@
   <dimension ref="A2:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,6 +539,11 @@
         <v>16</v>
       </c>
     </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
@@ -560,6 +571,9 @@
       </c>
       <c r="I14" t="s">
         <v>7</v>
+      </c>
+      <c r="J14" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>